<commit_message>
Rename the RACP lever in the webapp and set the alternate RACP to 9999
</commit_message>
<xml_diff>
--- a/InputData/elec/RACP/RPS Alternative Compliance Payment.xlsx
+++ b/InputData/elec/RACP/RPS Alternative Compliance Payment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\RACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087F45C0-E513-48B9-8A93-9538505CD438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0F855F-5615-4B6F-8C76-6AC2301E3C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>180*About!A12</f>
-        <v>135.63061614298562</v>
+        <v>9999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>